<commit_message>
Se agrega la ejecución para firefox
</commit_message>
<xml_diff>
--- a/data/RTM_for_QA_Tech_Challenge.xlsx
+++ b/data/RTM_for_QA_Tech_Challenge.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD23"/>
@@ -1430,6 +1430,302 @@
         </is>
       </c>
       <c r="N12" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Developer12</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>tester12</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Developer13</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>tester13</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Developer14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>tester14</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Developer15</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>tester15</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
         <is>
           <t>Or the output</t>
         </is>

</xml_diff>

<commit_message>
Termino de scenarios y documentacion de funciones
</commit_message>
<xml_diff>
--- a/data/RTM_for_QA_Tech_Challenge.xlsx
+++ b/data/RTM_for_QA_Tech_Challenge.xlsx
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD23"/>
@@ -1726,6 +1726,1264 @@
         </is>
       </c>
       <c r="N16" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Developer16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>tester16</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Developer17</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>tester17</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Developer18</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>tester18</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Developer19</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>tester19</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Developer20</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>tester20</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Developer21</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>tester21</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Developer22</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>tester22</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Developer23</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>tester23</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Developer24</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>tester24</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Developer25</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>tester25</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Developer26</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>tester26</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Developer27</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>tester27</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Developer28</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>tester28</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Developer29</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Validate SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text SELF PACED ONLINE TRAINING</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>tester29</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Developer30</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Validate IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text IN DEPTH MATERIAL</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>tester30</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Developer31</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Validate LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text LIFETIME INSTRUCTOR SUPPORT</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>tester31</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Or the output</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Developer32</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>landing Page</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Validate RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>1/4</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Pre-conditions</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Open Site
+Click in New window
+Validar text RESUME PREPARATION</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Text should be in site</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>tester32</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Text isnt in front of the site</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Test automation failed</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
         <is>
           <t>Or the output</t>
         </is>

</xml_diff>